<commit_message>
Corsi, Digit span: 엑셀 파일 수정
</commit_message>
<xml_diff>
--- a/template/Corsi.xlsx
+++ b/template/Corsi.xlsx
@@ -624,7 +624,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -662,9 +662,7 @@
         <f>SUM(F5:F20)</f>
         <v>0</v>
       </c>
-      <c r="D2" s="3">
-        <v>2</v>
-      </c>
+      <c r="D2" s="3"/>
       <c r="E2" s="5"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>